<commit_message>
populate table ipyb file updated and sqlite database with 5 tables and data uploaded
</commit_message>
<xml_diff>
--- a/SQLiteDB/2018-2019 Per Pupil Expenditures_db.xlsx
+++ b/SQLiteDB/2018-2019 Per Pupil Expenditures_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michellechampagne/Desktop/BOOTCAMP/UPenn-Data---Project-3/SQLiteDB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6FDD1ED-F281-9641-BA2D-05EACF16252E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61E3C43-EA5F-7240-AC69-D5E84E602465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46480" yWindow="6020" windowWidth="27640" windowHeight="16940" xr2:uid="{AC92E89F-EB58-D444-9DD6-7FB9EFFDF8A3}"/>
+    <workbookView xWindow="66440" yWindow="500" windowWidth="35580" windowHeight="21480" xr2:uid="{AC92E89F-EB58-D444-9DD6-7FB9EFFDF8A3}"/>
   </bookViews>
   <sheets>
     <sheet name="ESSA Exp per ADM LEA 2018-19" sheetId="1" r:id="rId1"/>
@@ -2702,17 +2702,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24DD4E54-BC33-EE4C-B747-7AB22469389E}">
   <dimension ref="A1:P674"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.5" style="1" bestFit="1" customWidth="1"/>

</xml_diff>